<commit_message>
Defect fixes: 1. There will be extraction result if we use default rules but no result if we write regex rules by ourselves. 2. Cannot extract metadata from content 3. Update metadata extraction list according to content classification matrix, instead of metadata class 4. Airline default rule cannot return metadata value 5. Cannot extract Month Metadata by default 6. Duplicated metadata extraction rule in CMVT 7. No Example in CMVT Metadata Extraction Rule 8 "&" becomes "&amps;" in Metadata XML file 9. Strange substring of the file name as a metadata (Content Subject) 10. Metadata XML encoding seems wrong 11. Metadata XML unexpectedly ends with a lot of mysterious spaces 12. source location cannot be deleted 13. Cannot extract metadata by regex 14. Cannot extract metadata from content - DOC-483 15. Snapshot_deleted is not updated for identified document instances
New Features
1. Generate Metadata XML by Document Class
2. Identify all document
3. Auto Filter in CMVT Reference File List
</commit_message>
<xml_diff>
--- a/MigrationManager/WebContent/resources/cmvt.xlsx
+++ b/MigrationManager/WebContent/resources/cmvt.xlsx
@@ -924,18 +924,6 @@
     <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -962,6 +950,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -9646,7 +9646,7 @@
   <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9662,10 +9662,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
@@ -9675,10 +9675,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -9686,59 +9686,59 @@
       <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
       <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
       <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="30"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -10484,8 +10484,7 @@
       <c r="G88" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A7:G7"/>
+  <mergeCells count="10">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
@@ -10512,7 +10511,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B106"/>
+  <dimension ref="A1:R106"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10520,74 +10519,91 @@
   <cols>
     <col min="1" max="1" width="118" style="19" customWidth="1"/>
     <col min="2" max="2" width="64.5703125" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="19"/>
+    <col min="3" max="18" width="18.140625" style="19" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="20"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
       <c r="B4" s="20"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="20"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="20"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="20"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
       <c r="B15" s="20"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="20"/>
     </row>

</xml_diff>